<commit_message>
EPBDS-3135 Check for return type in conditional array index.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/binding/ConditionalArrayIndexTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/binding/ConditionalArrayIndexTest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="18195" windowHeight="7740"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>String</t>
   </si>
@@ -134,13 +134,25 @@
   </si>
   <si>
     <t>return arrayOfDrivers[select first having  numMovingViolations == 0];</t>
+  </si>
+  <si>
+    <t>Method Driver[] errorSelect(Driver[] arrayOfDrivers)</t>
+  </si>
+  <si>
+    <t>return arrayOfDrivers[@ age = 20];</t>
+  </si>
+  <si>
+    <t>Method Driver[] errorSelectLiteral(Driver[] arrayOfDrivers)</t>
+  </si>
+  <si>
+    <t>return arrayOfDrivers[select all having  numMovingViolations = 0];</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,12 +564,6 @@
   </cellStyleXfs>
   <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -565,33 +571,6 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -627,9 +606,42 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -643,9 +655,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -683,7 +695,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -717,7 +729,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -752,10 +763,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -928,12 +938,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
@@ -943,277 +953,307 @@
     <col min="13" max="13" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:10">
+      <c r="B2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="F2" s="16" t="s">
+      <c r="C2" s="22"/>
+      <c r="F2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:10">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="2:10">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="14">
         <v>38</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="14">
         <v>17</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="15">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="2:10">
+      <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="2:10">
+      <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="2:10">
+      <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="14">
         <v>0</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="14">
         <v>0</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J8" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="2:10">
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="16">
         <v>1</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="14">
         <v>0</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="2:10">
+      <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="14">
         <v>0</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="14">
         <v>0</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10" s="15">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="2:10">
+      <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="31" t="s">
+      <c r="J11" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+    <row r="14" spans="2:10">
+      <c r="B14" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="F14" s="10" t="s">
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="F14" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="12"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="F15" s="13" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="31"/>
+      <c r="F15" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="F17" s="10" t="s">
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="F17" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="F18" s="13" t="s">
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
+      <c r="F18" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31"/>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="F21" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="27"/>
+      <c r="H21" s="28"/>
+    </row>
+    <row r="22" spans="2:8" ht="15" customHeight="1">
+      <c r="B22" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="31"/>
+      <c r="F22" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="30"/>
+      <c r="H22" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="F14:H14"/>
@@ -1222,8 +1262,6 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="F18:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added SelectFirst tests for Spreadsheet
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/binding/ConditionalArrayIndexTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/binding/ConditionalArrayIndexTest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="18195" windowHeight="7740"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="test" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>String</t>
   </si>
@@ -146,13 +146,49 @@
   </si>
   <si>
     <t>return arrayOfDrivers[select all having  numMovingViolations = 0];</t>
+  </si>
+  <si>
+    <t>SelectStep</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>=$SelectStep</t>
+  </si>
+  <si>
+    <t>Formula:Driver</t>
+  </si>
+  <si>
+    <t>Age:int</t>
+  </si>
+  <si>
+    <t>=maxAge</t>
+  </si>
+  <si>
+    <t>=dd[!@ age &lt; $Age]</t>
+  </si>
+  <si>
+    <t>Spreadsheet Driver checkSpreadsheet1(Driver[] dd, int maxAge)</t>
+  </si>
+  <si>
+    <t>Spreadsheet Driver checkSpreadsheet2(Driver[] dd, int dIndex)</t>
+  </si>
+  <si>
+    <t>Index:int</t>
+  </si>
+  <si>
+    <t>=dIndex</t>
+  </si>
+  <si>
+    <t>=dd[!@ name == testDrivers[$Index].name]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,7 +598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -606,6 +642,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -621,23 +675,9 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -729,6 +769,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -763,6 +804,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -938,36 +980,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:J22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27:I27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.5703125" customWidth="1"/>
+    <col min="8" max="8" width="35.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
     <col min="13" max="13" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:10">
-      <c r="B2" s="21" t="s">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="F2" s="23" t="s">
+      <c r="C2" s="28"/>
+      <c r="F2" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="25"/>
-    </row>
-    <row r="3" spans="2:10">
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -990,7 +1036,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +1059,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1036,7 +1082,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1059,7 +1105,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1128,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1105,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1128,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
@@ -1151,7 +1197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
@@ -1174,86 +1220,142 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="26" t="s">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28"/>
-      <c r="F14" s="26" t="s">
+      <c r="C14" s="25"/>
+      <c r="D14" s="26"/>
+      <c r="F14" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="B15" s="29" t="s">
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31"/>
-      <c r="F15" s="29" t="s">
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="F15" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="26" t="s">
+      <c r="G15" s="22"/>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
-      <c r="F17" s="26" t="s">
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+      <c r="F17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="29" t="s">
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="31"/>
-      <c r="F18" s="29" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="F18" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="31"/>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="26" t="s">
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
-      <c r="F21" s="26" t="s">
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
+      <c r="F21" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="27"/>
-      <c r="H21" s="28"/>
-    </row>
-    <row r="22" spans="2:8" ht="15" customHeight="1">
-      <c r="B22" s="29" t="s">
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+    </row>
+    <row r="22" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
-      <c r="F22" s="29" t="s">
+      <c r="C22" s="22"/>
+      <c r="D22" s="23"/>
+      <c r="F22" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="31"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="23"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="G27" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" t="s">
+        <v>47</v>
+      </c>
+      <c r="I28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
+  <mergeCells count="16">
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="G27:I27"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="F14:H14"/>
@@ -1262,6 +1364,12 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>